<commit_message>
- Added new Test Files - Introduced metric with LLM as judge - Added new metric to the benchmark
</commit_message>
<xml_diff>
--- a/core/src/test/resources/llm-bench/bird/queries.xlsx
+++ b/core/src/test/resources/llm-bench/bird/queries.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzoveltri/git/galois/core/src/test/resources/llm-bench/bird/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FA6A1C-D914-3F42-9D25-8D1597AF287F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D70CFB6-3961-1141-932F-F37B7E43E8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="queries" sheetId="2" r:id="rId1"/>
-    <sheet name="original" sheetId="3" r:id="rId2"/>
+    <sheet name="queries" sheetId="4" r:id="rId1"/>
+    <sheet name="queries-manual" sheetId="2" r:id="rId2"/>
+    <sheet name="original" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">original!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">original!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">queries!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'queries-manual'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="186">
   <si>
     <t>db_id</t>
   </si>
@@ -573,6 +575,21 @@
   </si>
   <si>
     <t>SELECT city FROM institution_details WHERE chronname = 'Rensselaer Polytechnic Institute';</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(T2.county) as county FROM state AS T1 INNER JOIN country AS T2 ON T1.abbreviation = T2.state WHERE T1.name = 'Virginia'</t>
+  </si>
+  <si>
+    <t>SELECT SUM(T2.population_2020) as population_2020 FROM country AS T1 INNER JOIN zip_data AS T2 ON T1.zip_code = T2.zip_code WHERE T1.county = 'ARECIBO'</t>
+  </si>
+  <si>
+    <t>SELECT T1.Area, COUNT(T3.Name) as Name FROM continent AS T1 INNER JOIN encompasses AS T2 ON T1.Name = T2.Continent INNER JOIN country AS T3 ON T3.Code = T2.Country WHERE T1.Name = 'Asia' GROUP BY T1.Name, T1.Area</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(T1.movie_id) as movie_id FROM movie AS T1 INNER JOIN movie_cast AS T2 ON T1.movie_id = T2.movie_id INNER JOIN person AS T3 ON T2.person_id = T3.person_id WHERE T3.person_name = 'Quentin Tarantino' AND CAST(SUBSTRING(T1.release_date,1,4) AS INT) = 1995</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(T3.id) as id FROM games AS T1 INNER JOIN games_competitor AS T2 ON T1.id = T2.games_id INNER JOIN person AS T3 ON T2.person_id = T3.id INNER JOIN person_region AS T4 ON T3.id = T4.person_id INNER JOIN noc_region AS T5 ON T4.region_id = T5.id WHERE T1.games_name = '2016 Summer' AND T5.region_name = 'China'</t>
   </si>
 </sst>
 </file>
@@ -856,10 +873,1802 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50513C55-97B3-8B47-930B-791F99A24CBA}">
+  <dimension ref="A1:C999"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B76" sqref="B76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="106.6640625" customWidth="1"/>
+    <col min="3" max="23" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
@@ -2658,7 +4467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA81987-170F-0641-81A0-9767FF9C828C}">
   <dimension ref="A1:C1000"/>
   <sheetViews>

</xml_diff>

<commit_message>
Commit experiment configuration with QATCH
</commit_message>
<xml_diff>
--- a/core/src/test/resources/llm-bench/bird/queries.xlsx
+++ b/core/src/test/resources/llm-bench/bird/queries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzoveltri/git/galois/core/src/test/resources/llm-bench/bird/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D70CFB6-3961-1141-932F-F37B7E43E8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75300BC4-BAF9-7343-90F4-C0EEADBE1529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="queries" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">original!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">queries!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">queries!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'queries-manual'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="199">
   <si>
     <t>db_id</t>
   </si>
@@ -590,6 +590,45 @@
   </si>
   <si>
     <t>SELECT COUNT(T3.id) as id FROM games AS T1 INNER JOIN games_competitor AS T2 ON T1.id = T2.games_id INNER JOIN person AS T3 ON T2.person_id = T3.id INNER JOIN person_region AS T4 ON T3.id = T4.person_id INNER JOIN noc_region AS T5 ON T4.region_id = T5.id WHERE T1.games_name = '2016 Summer' AND T5.region_name = 'China'</t>
+  </si>
+  <si>
+    <t>tuples</t>
+  </si>
+  <si>
+    <t>attrs</t>
+  </si>
+  <si>
+    <t>numerical conditions</t>
+  </si>
+  <si>
+    <t>categorical conditions</t>
+  </si>
+  <si>
+    <t>tables</t>
+  </si>
+  <si>
+    <t>aggr</t>
+  </si>
+  <si>
+    <t>join</t>
+  </si>
+  <si>
+    <t>distinct</t>
+  </si>
+  <si>
+    <t>group by</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>order by</t>
+  </si>
+  <si>
+    <t>nested</t>
+  </si>
+  <si>
+    <t>like</t>
   </si>
 </sst>
 </file>
@@ -626,7 +665,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -649,16 +688,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -874,32 +936,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50513C55-97B3-8B47-930B-791F99A24CBA}">
-  <dimension ref="A1:C999"/>
+  <dimension ref="A1:P999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B76" sqref="B76"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="106.6640625" customWidth="1"/>
-    <col min="3" max="23" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="113.33203125" style="5" customWidth="1"/>
+    <col min="3" max="24" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -909,8 +1010,41 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -920,8 +1054,41 @@
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>54</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -931,8 +1098,41 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -942,8 +1142,41 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -953,8 +1186,41 @@
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -964,8 +1230,41 @@
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>159</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -975,8 +1274,41 @@
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>399</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -986,8 +1318,41 @@
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -997,74 +1362,305 @@
       <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
@@ -1074,8 +1670,41 @@
       <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
@@ -1085,19 +1714,85 @@
       <c r="C18" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>159</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
@@ -1107,8 +1802,41 @@
       <c r="C20" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
@@ -1118,8 +1846,41 @@
       <c r="C21" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>44</v>
       </c>
@@ -1129,8 +1890,41 @@
       <c r="C22" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1140,8 +1934,41 @@
       <c r="C23" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
@@ -1151,8 +1978,41 @@
       <c r="C24" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
@@ -1162,8 +2022,41 @@
       <c r="C25" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
@@ -1173,8 +2066,41 @@
       <c r="C26" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
@@ -1184,8 +2110,41 @@
       <c r="C27" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
@@ -1195,8 +2154,41 @@
       <c r="C28" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
@@ -1206,8 +2198,41 @@
       <c r="C29" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>44</v>
       </c>
@@ -1217,8 +2242,41 @@
       <c r="C30" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -1228,8 +2286,41 @@
       <c r="C31" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
@@ -1239,8 +2330,41 @@
       <c r="C32" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -1250,8 +2374,41 @@
       <c r="C33" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>3</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -1261,8 +2418,41 @@
       <c r="C34" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
@@ -1272,8 +2462,41 @@
       <c r="C35" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>71</v>
       </c>
@@ -1283,8 +2506,41 @@
       <c r="C36" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>71</v>
       </c>
@@ -1294,8 +2550,41 @@
       <c r="C37" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>3</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>71</v>
       </c>
@@ -1305,8 +2594,41 @@
       <c r="C38" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>71</v>
       </c>
@@ -1316,8 +2638,41 @@
       <c r="C39" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>71</v>
       </c>
@@ -1327,8 +2682,41 @@
       <c r="C40" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>7</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>71</v>
       </c>
@@ -1338,8 +2726,41 @@
       <c r="C41" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>3</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>71</v>
       </c>
@@ -1349,8 +2770,41 @@
       <c r="C42" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>71</v>
       </c>
@@ -1360,8 +2814,41 @@
       <c r="C43" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>71</v>
       </c>
@@ -1371,8 +2858,41 @@
       <c r="C44" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>71</v>
       </c>
@@ -1382,8 +2902,41 @@
       <c r="C45" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>71</v>
       </c>
@@ -1393,8 +2946,41 @@
       <c r="C46" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>71</v>
       </c>
@@ -1404,8 +2990,41 @@
       <c r="C47" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>2</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>71</v>
       </c>
@@ -1415,8 +3034,41 @@
       <c r="C48" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>4</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>71</v>
       </c>
@@ -1426,8 +3078,41 @@
       <c r="C49" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>71</v>
       </c>
@@ -1437,8 +3122,41 @@
       <c r="C50" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>2</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>71</v>
       </c>
@@ -1448,8 +3166,41 @@
       <c r="C51" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>71</v>
       </c>
@@ -1459,8 +3210,41 @@
       <c r="C52" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>71</v>
       </c>
@@ -1470,8 +3254,44 @@
       <c r="C53" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <v>9</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>107</v>
       </c>
@@ -1481,162 +3301,663 @@
       <c r="C54" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="4" t="s">
         <v>112</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>4</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>5</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="4" t="s">
         <v>114</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>3</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>2</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="P56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="4" t="s">
         <v>116</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>4</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>2</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="4" t="s">
         <v>120</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>4</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>2</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="4" t="s">
         <v>122</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>3</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>4</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>2</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="4" t="s">
         <v>124</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>4</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>2</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="4" t="s">
         <v>184</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>3</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>2</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="4" t="s">
         <v>129</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>3</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>2</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="4" t="s">
         <v>185</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>5</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>6</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>4</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="4" t="s">
         <v>133</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>3</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>2</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="4" t="s">
         <v>135</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>3</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>2</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>2</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="4" t="s">
         <v>169</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>2</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="4" t="s">
         <v>139</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>3</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>3</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>2</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>140</v>
       </c>
@@ -1646,8 +3967,41 @@
       <c r="C69" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>2</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>140</v>
       </c>
@@ -1657,8 +4011,41 @@
       <c r="C70" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>2</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>140</v>
       </c>
@@ -1668,8 +4055,41 @@
       <c r="C71" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>140</v>
       </c>
@@ -1679,8 +4099,41 @@
       <c r="C72" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>148</v>
       </c>
@@ -1690,8 +4143,41 @@
       <c r="C73" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>148</v>
       </c>
@@ -1701,8 +4187,41 @@
       <c r="C74" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <v>3</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>2</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>3</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>148</v>
       </c>
@@ -1712,32 +4231,131 @@
       <c r="C75" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <v>51</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="4" t="s">
         <v>174</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>2</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>3</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76">
+        <v>1</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>2</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>3</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2658,7 +5276,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:N1" xr:uid="{50513C55-97B3-8B47-930B-791F99A24CBA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -2669,8 +5287,8 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added a unique TestBench for LLMs
</commit_message>
<xml_diff>
--- a/core/src/test/resources/llm-bench/bird/queries.xlsx
+++ b/core/src/test/resources/llm-bench/bird/queries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzoveltri/git/galois/core/src/test/resources/llm-bench/bird/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75300BC4-BAF9-7343-90F4-C0EEADBE1529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25835E27-82C4-C042-A392-02F7A3CA76DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="queries" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">original!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">queries!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">queries!$A$1:$P$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'queries-manual'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="201">
   <si>
     <t>db_id</t>
   </si>
@@ -629,6 +629,12 @@
   </si>
   <si>
     <t>like</t>
+  </si>
+  <si>
+    <t>attr numerical</t>
+  </si>
+  <si>
+    <t>attr categorical</t>
   </si>
 </sst>
 </file>
@@ -936,21 +942,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50513C55-97B3-8B47-930B-791F99A24CBA}">
-  <dimension ref="A1:P999"/>
+  <dimension ref="A1:R999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G81" sqref="G81:H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="113.33203125" style="5" customWidth="1"/>
-    <col min="3" max="24" width="10.6640625" customWidth="1"/>
+    <col min="3" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -966,41 +972,47 @@
       <c r="E1" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1017,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1026,16 +1038,16 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1043,8 +1055,14 @@
       <c r="N2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1061,34 +1079,40 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>3</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1105,13 +1129,13 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1120,10 +1144,10 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -1131,8 +1155,14 @@
       <c r="N4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1149,34 +1179,40 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1193,16 +1229,16 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1211,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1219,8 +1255,14 @@
       <c r="N6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1237,10 +1279,10 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -1255,16 +1297,22 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1281,13 +1329,13 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1296,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -1305,10 +1353,16 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1325,25 +1379,25 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1351,8 +1405,14 @@
       <c r="N9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -1369,34 +1429,40 @@
         <v>1</v>
       </c>
       <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>3</v>
       </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
       <c r="I10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10">
         <v>2</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -1413,25 +1479,25 @@
         <v>1</v>
       </c>
       <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>3</v>
       </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
       <c r="I11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1439,8 +1505,14 @@
       <c r="N11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1457,34 +1529,40 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1501,16 +1579,16 @@
         <v>1</v>
       </c>
       <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>3</v>
       </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
       <c r="I13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13">
         <v>2</v>
@@ -1519,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1527,8 +1605,14 @@
       <c r="N13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -1545,25 +1629,25 @@
         <v>1</v>
       </c>
       <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>3</v>
       </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
       <c r="I14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1571,8 +1655,14 @@
       <c r="N14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -1589,34 +1679,40 @@
         <v>1</v>
       </c>
       <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <v>3</v>
       </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
       <c r="I15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1633,16 +1729,16 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1651,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -1659,8 +1755,14 @@
       <c r="N16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
@@ -1677,10 +1779,10 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1689,7 +1791,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -1703,8 +1805,14 @@
       <c r="N17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
@@ -1721,10 +1829,10 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1733,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1747,8 +1855,14 @@
       <c r="N18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -1765,19 +1879,19 @@
         <v>1</v>
       </c>
       <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
         <v>3</v>
       </c>
-      <c r="G19">
-        <v>2</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
       <c r="I19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1791,8 +1905,14 @@
       <c r="N19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
@@ -1818,13 +1938,13 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -1835,8 +1955,14 @@
       <c r="N20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
@@ -1856,19 +1982,19 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -1879,8 +2005,14 @@
       <c r="N21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>44</v>
       </c>
@@ -1897,10 +2029,10 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <v>2</v>
@@ -1909,13 +2041,13 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -1923,8 +2055,14 @@
       <c r="N22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1941,10 +2079,10 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -1953,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -1967,8 +2105,14 @@
       <c r="N23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
@@ -1985,10 +2129,10 @@
         <v>3</v>
       </c>
       <c r="F24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24">
         <v>2</v>
@@ -1997,13 +2141,13 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -2011,8 +2155,14 @@
       <c r="N24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
@@ -2029,20 +2179,20 @@
         <v>1</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
         <v>3</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
       <c r="K25">
         <v>0</v>
       </c>
@@ -2055,8 +2205,14 @@
       <c r="N25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
@@ -2073,10 +2229,10 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -2085,7 +2241,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -2099,8 +2255,14 @@
       <c r="N26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
@@ -2117,7 +2279,7 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -2126,16 +2288,16 @@
         <v>2</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -2143,8 +2305,14 @@
       <c r="N27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
@@ -2161,10 +2329,10 @@
         <v>1</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -2173,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -2187,8 +2355,14 @@
       <c r="N28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
@@ -2205,25 +2379,25 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
         <v>3</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>1</v>
-      </c>
       <c r="K29">
         <v>0</v>
       </c>
       <c r="L29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -2231,8 +2405,14 @@
       <c r="N29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>44</v>
       </c>
@@ -2249,10 +2429,10 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -2261,7 +2441,7 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -2275,8 +2455,14 @@
       <c r="N30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -2293,10 +2479,10 @@
         <v>1</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -2305,7 +2491,7 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -2319,8 +2505,14 @@
       <c r="N31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
@@ -2337,10 +2529,10 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32">
         <v>2</v>
@@ -2349,13 +2541,13 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K32">
         <v>0</v>
       </c>
       <c r="L32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -2363,8 +2555,14 @@
       <c r="N32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -2381,25 +2579,25 @@
         <v>1</v>
       </c>
       <c r="F33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
         <v>3</v>
       </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
       <c r="K33">
         <v>0</v>
       </c>
       <c r="L33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -2407,8 +2605,14 @@
       <c r="N33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -2425,10 +2629,10 @@
         <v>1</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -2437,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -2451,8 +2655,14 @@
       <c r="N34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
@@ -2469,10 +2679,10 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -2481,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -2495,8 +2705,14 @@
       <c r="N35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>71</v>
       </c>
@@ -2513,10 +2729,10 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -2525,13 +2741,13 @@
         <v>0</v>
       </c>
       <c r="J36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K36">
         <v>0</v>
       </c>
       <c r="L36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36">
         <v>0</v>
@@ -2539,8 +2755,14 @@
       <c r="N36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>71</v>
       </c>
@@ -2557,7 +2779,7 @@
         <v>1</v>
       </c>
       <c r="F37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2569,13 +2791,13 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K37">
         <v>0</v>
       </c>
       <c r="L37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M37">
         <v>0</v>
@@ -2583,8 +2805,14 @@
       <c r="N37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>71</v>
       </c>
@@ -2601,10 +2829,10 @@
         <v>1</v>
       </c>
       <c r="F38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>2</v>
@@ -2613,22 +2841,28 @@
         <v>0</v>
       </c>
       <c r="J38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>71</v>
       </c>
@@ -2645,25 +2879,25 @@
         <v>1</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
         <v>3</v>
       </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
       <c r="K39">
         <v>0</v>
       </c>
       <c r="L39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39">
         <v>0</v>
@@ -2671,8 +2905,14 @@
       <c r="N39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>71</v>
       </c>
@@ -2689,10 +2929,10 @@
         <v>1</v>
       </c>
       <c r="F40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <v>3</v>
@@ -2701,13 +2941,13 @@
         <v>0</v>
       </c>
       <c r="J40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K40">
         <v>0</v>
       </c>
       <c r="L40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M40">
         <v>0</v>
@@ -2715,8 +2955,14 @@
       <c r="N40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>71</v>
       </c>
@@ -2733,7 +2979,7 @@
         <v>2</v>
       </c>
       <c r="F41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2745,22 +2991,28 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M41">
         <v>0</v>
       </c>
       <c r="N41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>71</v>
       </c>
@@ -2777,10 +3029,10 @@
         <v>2</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -2789,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="J42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -2803,8 +3055,14 @@
       <c r="N42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>71</v>
       </c>
@@ -2821,10 +3079,10 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -2833,7 +3091,7 @@
         <v>0</v>
       </c>
       <c r="J43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -2847,8 +3105,14 @@
       <c r="N43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>71</v>
       </c>
@@ -2868,7 +3132,7 @@
         <v>1</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -2877,7 +3141,7 @@
         <v>0</v>
       </c>
       <c r="J44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44">
         <v>0</v>
@@ -2886,13 +3150,19 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>71</v>
       </c>
@@ -2915,13 +3185,13 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I45">
         <v>0</v>
       </c>
       <c r="J45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K45">
         <v>0</v>
@@ -2935,8 +3205,14 @@
       <c r="N45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>71</v>
       </c>
@@ -2953,10 +3229,10 @@
         <v>1</v>
       </c>
       <c r="F46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
         <v>2</v>
@@ -2965,7 +3241,7 @@
         <v>0</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -2979,8 +3255,14 @@
       <c r="N46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>71</v>
       </c>
@@ -2997,10 +3279,10 @@
         <v>1</v>
       </c>
       <c r="F47">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
         <v>3</v>
@@ -3009,22 +3291,28 @@
         <v>0</v>
       </c>
       <c r="J47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K47">
         <v>0</v>
       </c>
       <c r="L47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>71</v>
       </c>
@@ -3041,25 +3329,25 @@
         <v>1</v>
       </c>
       <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
         <v>3</v>
       </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
         <v>4</v>
       </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-      <c r="J48">
-        <v>2</v>
-      </c>
       <c r="K48">
         <v>0</v>
       </c>
       <c r="L48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M48">
         <v>0</v>
@@ -3067,8 +3355,14 @@
       <c r="N48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>71</v>
       </c>
@@ -3085,10 +3379,10 @@
         <v>1</v>
       </c>
       <c r="F49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <v>2</v>
@@ -3097,13 +3391,13 @@
         <v>0</v>
       </c>
       <c r="J49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K49">
         <v>0</v>
       </c>
       <c r="L49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49">
         <v>0</v>
@@ -3111,8 +3405,14 @@
       <c r="N49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>71</v>
       </c>
@@ -3129,25 +3429,25 @@
         <v>1</v>
       </c>
       <c r="F50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K50">
         <v>0</v>
       </c>
       <c r="L50">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M50">
         <v>0</v>
@@ -3155,8 +3455,14 @@
       <c r="N50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>71</v>
       </c>
@@ -3173,7 +3479,7 @@
         <v>1</v>
       </c>
       <c r="F51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -3182,10 +3488,10 @@
         <v>1</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51">
         <v>0</v>
@@ -3199,8 +3505,14 @@
       <c r="N51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>71</v>
       </c>
@@ -3217,10 +3529,10 @@
         <v>1</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -3229,7 +3541,7 @@
         <v>0</v>
       </c>
       <c r="J52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52">
         <v>0</v>
@@ -3238,13 +3550,19 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="P52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>71</v>
       </c>
@@ -3261,10 +3579,10 @@
         <v>1</v>
       </c>
       <c r="F53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53">
         <v>2</v>
@@ -3273,7 +3591,7 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -3288,10 +3606,16 @@
         <v>0</v>
       </c>
       <c r="O53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>107</v>
       </c>
@@ -3308,16 +3632,16 @@
         <v>1</v>
       </c>
       <c r="F54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G54">
         <v>1</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54">
         <v>1</v>
@@ -3326,7 +3650,7 @@
         <v>0</v>
       </c>
       <c r="L54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54">
         <v>0</v>
@@ -3334,8 +3658,14 @@
       <c r="N54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>110</v>
       </c>
@@ -3352,34 +3682,40 @@
         <v>1</v>
       </c>
       <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
         <v>4</v>
       </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
         <v>5</v>
       </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-      <c r="J55">
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
         <v>3</v>
       </c>
-      <c r="K55">
-        <v>0</v>
-      </c>
-      <c r="L55">
-        <v>0</v>
-      </c>
       <c r="M55">
         <v>0</v>
       </c>
       <c r="N55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>110</v>
       </c>
@@ -3396,10 +3732,10 @@
         <v>1</v>
       </c>
       <c r="F56">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56">
         <v>3</v>
@@ -3408,25 +3744,31 @@
         <v>0</v>
       </c>
       <c r="J56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K56">
         <v>0</v>
       </c>
       <c r="L56">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
         <v>1</v>
       </c>
       <c r="P56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="R56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>110</v>
       </c>
@@ -3443,25 +3785,25 @@
         <v>1</v>
       </c>
       <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
         <v>3</v>
       </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
         <v>4</v>
       </c>
-      <c r="I57">
-        <v>0</v>
-      </c>
-      <c r="J57">
-        <v>2</v>
-      </c>
       <c r="K57">
         <v>0</v>
       </c>
       <c r="L57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M57">
         <v>0</v>
@@ -3469,8 +3811,14 @@
       <c r="N57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>110</v>
       </c>
@@ -3487,10 +3835,10 @@
         <v>1</v>
       </c>
       <c r="F58">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58">
         <v>2</v>
@@ -3499,22 +3847,28 @@
         <v>0</v>
       </c>
       <c r="J58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="O58">
+        <v>0</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>110</v>
       </c>
@@ -3531,25 +3885,25 @@
         <v>1</v>
       </c>
       <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
         <v>3</v>
       </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
         <v>4</v>
       </c>
-      <c r="I59">
-        <v>0</v>
-      </c>
-      <c r="J59">
-        <v>2</v>
-      </c>
       <c r="K59">
         <v>0</v>
       </c>
       <c r="L59">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M59">
         <v>0</v>
@@ -3557,11 +3911,17 @@
       <c r="N59">
         <v>0</v>
       </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
       <c r="P59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="R59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>110</v>
       </c>
@@ -3578,25 +3938,25 @@
         <v>1</v>
       </c>
       <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
         <v>3</v>
       </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
         <v>4</v>
       </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-      <c r="J60">
-        <v>2</v>
-      </c>
       <c r="K60">
         <v>0</v>
       </c>
       <c r="L60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M60">
         <v>0</v>
@@ -3604,8 +3964,14 @@
       <c r="N60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>110</v>
       </c>
@@ -3622,25 +3988,25 @@
         <v>1</v>
       </c>
       <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61">
         <v>3</v>
       </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
         <v>4</v>
       </c>
-      <c r="I61">
-        <v>0</v>
-      </c>
-      <c r="J61">
-        <v>2</v>
-      </c>
       <c r="K61">
         <v>0</v>
       </c>
       <c r="L61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M61">
         <v>0</v>
@@ -3648,8 +4014,14 @@
       <c r="N61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>110</v>
       </c>
@@ -3666,10 +4038,10 @@
         <v>1</v>
       </c>
       <c r="F62">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62">
         <v>3</v>
@@ -3678,13 +4050,13 @@
         <v>1</v>
       </c>
       <c r="J62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M62">
         <v>0</v>
@@ -3692,8 +4064,14 @@
       <c r="N62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>127</v>
       </c>
@@ -3710,10 +4088,10 @@
         <v>1</v>
       </c>
       <c r="F63">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63">
         <v>3</v>
@@ -3722,13 +4100,13 @@
         <v>0</v>
       </c>
       <c r="J63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K63">
         <v>0</v>
       </c>
       <c r="L63">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M63">
         <v>0</v>
@@ -3736,8 +4114,14 @@
       <c r="N63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>127</v>
       </c>
@@ -3754,34 +4138,40 @@
         <v>1</v>
       </c>
       <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
         <v>5</v>
       </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-      <c r="H64">
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
         <v>6</v>
       </c>
-      <c r="I64">
-        <v>1</v>
-      </c>
-      <c r="J64">
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
         <v>4</v>
       </c>
-      <c r="K64">
-        <v>0</v>
-      </c>
-      <c r="L64">
-        <v>0</v>
-      </c>
       <c r="M64">
         <v>0</v>
       </c>
       <c r="N64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>127</v>
       </c>
@@ -3798,7 +4188,7 @@
         <v>1</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -3810,13 +4200,13 @@
         <v>0</v>
       </c>
       <c r="J65">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K65">
         <v>0</v>
       </c>
       <c r="L65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M65">
         <v>0</v>
@@ -3824,8 +4214,14 @@
       <c r="N65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>127</v>
       </c>
@@ -3842,16 +4238,16 @@
         <v>1</v>
       </c>
       <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
         <v>3</v>
       </c>
-      <c r="G66">
-        <v>1</v>
-      </c>
-      <c r="H66">
-        <v>2</v>
-      </c>
       <c r="I66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J66">
         <v>2</v>
@@ -3860,7 +4256,7 @@
         <v>0</v>
       </c>
       <c r="L66">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M66">
         <v>0</v>
@@ -3868,8 +4264,14 @@
       <c r="N66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>127</v>
       </c>
@@ -3886,7 +4288,7 @@
         <v>1</v>
       </c>
       <c r="F67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -3898,10 +4300,10 @@
         <v>1</v>
       </c>
       <c r="J67">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L67">
         <v>1</v>
@@ -3910,10 +4312,16 @@
         <v>0</v>
       </c>
       <c r="N67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>127</v>
       </c>
@@ -3930,10 +4338,10 @@
         <v>1</v>
       </c>
       <c r="F68">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68">
         <v>3</v>
@@ -3942,13 +4350,13 @@
         <v>0</v>
       </c>
       <c r="J68">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K68">
         <v>0</v>
       </c>
       <c r="L68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M68">
         <v>0</v>
@@ -3956,8 +4364,14 @@
       <c r="N68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>140</v>
       </c>
@@ -3974,10 +4388,10 @@
         <v>1</v>
       </c>
       <c r="F69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69">
         <v>2</v>
@@ -3986,13 +4400,13 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K69">
         <v>0</v>
       </c>
       <c r="L69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M69">
         <v>0</v>
@@ -4000,8 +4414,14 @@
       <c r="N69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>140</v>
       </c>
@@ -4018,10 +4438,10 @@
         <v>1</v>
       </c>
       <c r="F70">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70">
         <v>2</v>
@@ -4030,13 +4450,13 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K70">
         <v>0</v>
       </c>
       <c r="L70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M70">
         <v>0</v>
@@ -4044,8 +4464,14 @@
       <c r="N70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O70">
+        <v>0</v>
+      </c>
+      <c r="P70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>140</v>
       </c>
@@ -4062,10 +4488,10 @@
         <v>1</v>
       </c>
       <c r="F71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71">
         <v>2</v>
@@ -4074,13 +4500,13 @@
         <v>0</v>
       </c>
       <c r="J71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K71">
         <v>0</v>
       </c>
       <c r="L71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M71">
         <v>0</v>
@@ -4088,8 +4514,14 @@
       <c r="N71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>140</v>
       </c>
@@ -4118,7 +4550,7 @@
         <v>0</v>
       </c>
       <c r="J72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K72">
         <v>0</v>
@@ -4132,8 +4564,14 @@
       <c r="N72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="P72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>148</v>
       </c>
@@ -4150,16 +4588,16 @@
         <v>1</v>
       </c>
       <c r="F73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73">
         <v>1</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -4176,8 +4614,14 @@
       <c r="N73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O73">
+        <v>0</v>
+      </c>
+      <c r="P73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>148</v>
       </c>
@@ -4194,25 +4638,25 @@
         <v>1</v>
       </c>
       <c r="F74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
         <v>3</v>
       </c>
-      <c r="I74">
-        <v>0</v>
-      </c>
-      <c r="J74">
-        <v>1</v>
-      </c>
       <c r="K74">
         <v>0</v>
       </c>
       <c r="L74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M74">
         <v>0</v>
@@ -4220,8 +4664,14 @@
       <c r="N74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O74">
+        <v>0</v>
+      </c>
+      <c r="P74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>148</v>
       </c>
@@ -4238,10 +4688,10 @@
         <v>1</v>
       </c>
       <c r="F75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -4250,7 +4700,7 @@
         <v>0</v>
       </c>
       <c r="J75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K75">
         <v>0</v>
@@ -4264,8 +4714,14 @@
       <c r="N75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="O75">
+        <v>0</v>
+      </c>
+      <c r="P75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>148</v>
       </c>
@@ -4282,34 +4738,40 @@
         <v>1</v>
       </c>
       <c r="F76">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76">
+        <v>2</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
         <v>3</v>
       </c>
-      <c r="I76">
-        <v>0</v>
-      </c>
-      <c r="J76">
-        <v>1</v>
-      </c>
       <c r="K76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="O76">
+        <v>0</v>
+      </c>
+      <c r="P76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>148</v>
       </c>
@@ -4326,25 +4788,25 @@
         <v>1</v>
       </c>
       <c r="F77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H77">
+        <v>2</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
         <v>3</v>
       </c>
-      <c r="I77">
-        <v>0</v>
-      </c>
-      <c r="J77">
-        <v>1</v>
-      </c>
       <c r="K77">
         <v>0</v>
       </c>
       <c r="L77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M77">
         <v>0</v>
@@ -4352,10 +4814,16 @@
       <c r="N77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="O77">
+        <v>0</v>
+      </c>
+      <c r="P77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5276,7 +5744,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{50513C55-97B3-8B47-930B-791F99A24CBA}"/>
+  <autoFilter ref="A1:P1" xr:uid="{50513C55-97B3-8B47-930B-791F99A24CBA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -5286,7 +5754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>

</xml_diff>